<commit_message>
added data in the excel
</commit_message>
<xml_diff>
--- a/src/test/resources/config/NewEnquiryWeb.xlsx
+++ b/src/test/resources/config/NewEnquiryWeb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6F9A3C-60F8-49C1-9860-105E75B47479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89488F91-CF24-4F75-9889-5C50E2B5C859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enquiry Lead Creation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="252">
   <si>
     <t>custType</t>
   </si>
@@ -225,12 +225,6 @@
     <t>Customer reference</t>
   </si>
   <si>
-    <t>NEW I20</t>
-  </si>
-  <si>
-    <t>Petrol</t>
-  </si>
-  <si>
     <t>800000</t>
   </si>
   <si>
@@ -591,48 +585,6 @@
     <t>empName</t>
   </si>
   <si>
-    <t>MALPC812LNM362012</t>
-  </si>
-  <si>
-    <t>10291</t>
-  </si>
-  <si>
-    <t>Karingu Anil Kumar</t>
-  </si>
-  <si>
-    <t>MALBJ512LNM154069</t>
-  </si>
-  <si>
-    <t>6455</t>
-  </si>
-  <si>
-    <t>MALPA813LNM355396</t>
-  </si>
-  <si>
-    <t>14343</t>
-  </si>
-  <si>
-    <t>Karingula Umesh</t>
-  </si>
-  <si>
-    <t>nextFollowupType</t>
-  </si>
-  <si>
-    <t>nextFollowupTime</t>
-  </si>
-  <si>
-    <t>tdOffer</t>
-  </si>
-  <si>
-    <t>fuel_type</t>
-  </si>
-  <si>
-    <t>vin_number</t>
-  </si>
-  <si>
-    <t>transmission_type</t>
-  </si>
-  <si>
     <t>test_drive_datetime</t>
   </si>
   <si>
@@ -642,36 +594,9 @@
     <t>followupRemarks</t>
   </si>
   <si>
-    <t>9121412109</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>1.0 T  Asta (O) DCT</t>
-  </si>
-  <si>
-    <t>Manual</t>
-  </si>
-  <si>
     <t>2023-06-05 10:56:00</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>9989912727</t>
-  </si>
-  <si>
-    <t>ALCAZAR</t>
-  </si>
-  <si>
-    <t>Signature (O) AT (6STR) DT PTRL</t>
-  </si>
-  <si>
-    <t>Automatic</t>
-  </si>
-  <si>
     <t>2023-06-15 10:04:00</t>
   </si>
   <si>
@@ -765,20 +690,107 @@
     <t>Whatsapp Blast</t>
   </si>
   <si>
-    <t>nand55@gmail.com</t>
-  </si>
-  <si>
-    <t>Jeevan9@gmail.com</t>
-  </si>
-  <si>
-    <t>Kumarraju@gmail.com</t>
+    <t>MALB351CYRM593531</t>
+  </si>
+  <si>
+    <t>4TH YEAR OR UP TO 80,000 KM EXTENDED WARRANTY</t>
+  </si>
+  <si>
+    <t>CHENIGACHERLA SAMPATH RAJ</t>
+  </si>
+  <si>
+    <t>MALBH512TRM338094</t>
+  </si>
+  <si>
+    <t>MALBJ512LRM341076</t>
+  </si>
+  <si>
+    <t>A BHARATH</t>
+  </si>
+  <si>
+    <t>AURA / EXTER - 3 YEARS OR UPTO 45,000 KM SHIELD OF TRUST PACKAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHENIGACHERLA SAMPATH RAJ </t>
+  </si>
+  <si>
+    <t>MALPA812LRM104432</t>
+  </si>
+  <si>
+    <t>AJAY PULIPATI</t>
+  </si>
+  <si>
+    <t>nandKuamr@gmail.com</t>
+  </si>
+  <si>
+    <t>JeevanSatya@gmail.com</t>
+  </si>
+  <si>
+    <t>KumarRana@gmail.com</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>TDOffer</t>
+  </si>
+  <si>
+    <t>TDVin</t>
+  </si>
+  <si>
+    <t>DepositCertificate</t>
+  </si>
+  <si>
+    <t>NextFollowUptime</t>
+  </si>
+  <si>
+    <t>TextFollow</t>
+  </si>
+  <si>
+    <t>FollowUptype</t>
+  </si>
+  <si>
+    <t>nextFollowUpType</t>
+  </si>
+  <si>
+    <t>EnquiryTypeValue</t>
+  </si>
+  <si>
+    <t>MALB551CYPM400978-Grand i10 NIOS</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Need to check</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Home Visit</t>
+  </si>
+  <si>
+    <t>Warm</t>
+  </si>
+  <si>
+    <t>Video Conference</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Refused</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -813,6 +825,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFE3E3E3"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -859,15 +890,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -886,14 +918,20 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{1A14863E-3F93-4E1E-B9B2-96E27A5F7083}"/>
     <cellStyle name="Normal 3" xfId="5" xr:uid="{D924B725-4337-41A0-BA6F-0F6624E16348}"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{B33B7A2C-F9E1-47B4-9311-86F54F1C475B}"/>
     <cellStyle name="Normal 5" xfId="2" xr:uid="{E79EB5CD-0A5D-4B75-8D8D-7ADBC584F316}"/>
+    <cellStyle name="Normal 6" xfId="6" xr:uid="{EB86B3C0-D20E-473E-BB9B-5A64859722BC}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1207,16 +1245,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1356,24 +1394,24 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:46" ht="25">
       <c r="A2" s="1" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
       <c r="C2">
-        <v>9551457237</v>
+        <v>9534357137</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="E2" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="F2" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="G2" t="s">
         <v>48</v>
@@ -1397,49 +1435,49 @@
         <v>47</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="P2" t="s">
         <v>53</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="R2" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="X2" t="s">
         <v>54</v>
       </c>
       <c r="Y2" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="Z2" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="AE2" t="s">
         <v>55</v>
@@ -1457,18 +1495,18 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:46" ht="37.5">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="C3">
-        <v>8251203177</v>
+        <v>9251456177</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="F3" t="s">
         <v>48</v>
@@ -1504,49 +1542,49 @@
         <v>53</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="R3" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="X3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Y3" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="Z3" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="AC3" s="6" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="AD3" s="6" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="AE3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AG3" t="s">
         <v>57</v>
@@ -1555,24 +1593,24 @@
         <v>46</v>
       </c>
       <c r="AT3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:46" ht="25" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" ht="25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
       <c r="C4">
-        <v>9752033712</v>
+        <v>8752123712</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="E4" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="F4" t="s">
         <v>48</v>
@@ -1608,49 +1646,49 @@
         <v>53</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="R4" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
       <c r="X4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Y4" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="Z4" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="AE4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AG4" t="s">
         <v>57</v>
       </c>
       <c r="AS4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AT4" t="s">
         <v>58</v>
@@ -1672,26 +1710,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" t="s">
-        <v>77</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -1712,151 +1750,151 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" t="s">
         <v>78</v>
       </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c r="O1" t="s">
+      <c r="B2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>81</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>82</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" t="s">
-        <v>86</v>
       </c>
       <c r="G2" t="s">
         <v>48</v>
       </c>
       <c r="H2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
         <v>87</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>88</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>89</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>90</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>91</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>92</v>
       </c>
-      <c r="N2" t="s">
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
         <v>93</v>
       </c>
-      <c r="O2" t="s">
+      <c r="B3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>95</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>96</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>97</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>98</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>99</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>100</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>101</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>102</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>103</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>104</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>105</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>106</v>
       </c>
-      <c r="N3" t="s">
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
         <v>107</v>
       </c>
-      <c r="O3" t="s">
+      <c r="B4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>109</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>110</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>111</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>112</v>
-      </c>
-      <c r="E4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4" t="s">
-        <v>114</v>
       </c>
       <c r="G4" t="s">
         <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K4" t="s">
         <v>115</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>116</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>117</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>118</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>119</v>
-      </c>
-      <c r="N4" t="s">
-        <v>120</v>
-      </c>
-      <c r="O4" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1870,287 +1908,287 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
         <v>122</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>123</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>124</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>125</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>126</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>130</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>131</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>132</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>133</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>134</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>135</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>136</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>137</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>138</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>139</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>140</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>141</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>142</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>143</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>144</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>145</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>146</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>147</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>148</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>149</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>150</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" t="s">
         <v>151</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="B2" t="s">
         <v>152</v>
       </c>
-      <c r="AG1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
         <v>153</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>154</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>155</v>
       </c>
-      <c r="E2" t="s">
+      <c r="O2" t="s">
         <v>156</v>
       </c>
-      <c r="F2" t="s">
+      <c r="P2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>156</v>
+      </c>
+      <c r="R2" t="s">
         <v>157</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
+        <v>157</v>
+      </c>
+      <c r="T2" t="s">
         <v>158</v>
       </c>
-      <c r="P2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>158</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>159</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
+        <v>160</v>
+      </c>
+      <c r="W2" t="s">
+        <v>161</v>
+      </c>
+      <c r="X2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" t="s">
+        <v>168</v>
+      </c>
+      <c r="O3" t="s">
+        <v>156</v>
+      </c>
+      <c r="P3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>156</v>
+      </c>
+      <c r="R3" t="s">
+        <v>169</v>
+      </c>
+      <c r="S3" t="s">
+        <v>169</v>
+      </c>
+      <c r="T3" t="s">
+        <v>170</v>
+      </c>
+      <c r="U3" t="s">
         <v>159</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V3" t="s">
         <v>160</v>
       </c>
-      <c r="U2" t="s">
-        <v>161</v>
-      </c>
-      <c r="V2" t="s">
-        <v>162</v>
-      </c>
-      <c r="W2" t="s">
-        <v>163</v>
-      </c>
-      <c r="X2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="W3" t="s">
+        <v>171</v>
+      </c>
+      <c r="X3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC3" t="s">
         <v>164</v>
       </c>
-      <c r="Z2" t="s">
-        <v>165</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G3" t="s">
-        <v>170</v>
-      </c>
-      <c r="O3" t="s">
-        <v>158</v>
-      </c>
-      <c r="P3" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>158</v>
-      </c>
-      <c r="R3" t="s">
-        <v>171</v>
-      </c>
-      <c r="S3" t="s">
-        <v>171</v>
-      </c>
-      <c r="T3" t="s">
-        <v>172</v>
-      </c>
-      <c r="U3" t="s">
-        <v>161</v>
-      </c>
-      <c r="V3" t="s">
-        <v>162</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="AG3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" t="s">
         <v>173</v>
       </c>
-      <c r="X3" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" t="s">
         <v>174</v>
       </c>
-      <c r="Z3" t="s">
-        <v>158</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="F4" t="s">
         <v>175</v>
       </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="O4" t="s">
+        <v>156</v>
+      </c>
+      <c r="P4" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>156</v>
+      </c>
+      <c r="R4" t="s">
         <v>176</v>
       </c>
-      <c r="F4" t="s">
+      <c r="S4" t="s">
+        <v>176</v>
+      </c>
+      <c r="T4" t="s">
         <v>177</v>
       </c>
-      <c r="O4" t="s">
-        <v>158</v>
-      </c>
-      <c r="P4" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>158</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="U4" t="s">
+        <v>159</v>
+      </c>
+      <c r="V4" t="s">
+        <v>160</v>
+      </c>
+      <c r="W4" t="s">
         <v>178</v>
       </c>
-      <c r="S4" t="s">
-        <v>178</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="X4" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z4" t="s">
         <v>179</v>
       </c>
-      <c r="U4" t="s">
-        <v>161</v>
-      </c>
-      <c r="V4" t="s">
-        <v>162</v>
-      </c>
-      <c r="W4" t="s">
-        <v>180</v>
-      </c>
-      <c r="X4" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>181</v>
-      </c>
       <c r="AC4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AG4" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2160,91 +2198,92 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="31.1796875" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" customWidth="1"/>
+    <col min="3" max="3" width="47.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="22.08984375" customWidth="1"/>
+    <col min="6" max="6" width="28.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
         <v>182</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>183</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>184</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>185</v>
       </c>
-      <c r="E1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F2" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F3" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F4" t="s">
-        <v>195</v>
-      </c>
+      <c r="F4" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G4" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2253,77 +2292,98 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="23.90625" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" customWidth="1"/>
+    <col min="6" max="6" width="25.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>199</v>
-      </c>
-      <c r="I1" t="s">
-        <v>200</v>
-      </c>
-      <c r="J1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K1" t="s">
-        <v>202</v>
+    <row r="1" spans="1:13">
+      <c r="A1" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>242</v>
       </c>
       <c r="L1" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="M1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" t="s">
-        <v>207</v>
-      </c>
-      <c r="H2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" t="s">
-        <v>208</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="11">
+        <v>9885588888</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" s="14">
+        <v>45682.451388888898</v>
+      </c>
+      <c r="F2" s="14">
+        <v>45668.020833333299</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>248</v>
       </c>
       <c r="K2" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="L2" t="s">
         <v>58</v>
@@ -2332,30 +2392,37 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" t="s">
-        <v>207</v>
-      </c>
-      <c r="H3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" t="s">
-        <v>208</v>
+    <row r="3" spans="1:13">
+      <c r="A3" s="11">
+        <v>9720243505</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" s="14">
+        <v>45672.493055555598</v>
+      </c>
+      <c r="F3" s="14">
+        <v>45669.020833333299</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>248</v>
       </c>
       <c r="K3" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="L3" t="s">
         <v>58</v>
@@ -2364,30 +2431,25 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" t="s">
-        <v>210</v>
-      </c>
-      <c r="F4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" t="s">
-        <v>214</v>
-      </c>
+    <row r="4" spans="1:13">
+      <c r="A4" s="11">
+        <v>9664587887</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
       <c r="K4" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="L4" t="s">
         <v>58</v>
@@ -2395,6 +2457,58 @@
       <c r="M4" t="s">
         <v>58</v>
       </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="11">
+        <v>9676562365</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="11">
+        <v>9959267961</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="11">
+        <v>7865897654</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2403,66 +2517,78 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="37.26953125" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="59.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" customWidth="1"/>
+    <col min="5" max="5" width="30.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" t="s">
         <v>185</v>
       </c>
-      <c r="C1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E2" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E3" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D4" t="s">
-        <v>195</v>
+      <c r="E4" s="9" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>